<commit_message>
create dynamic date (unfinish)
</commit_message>
<xml_diff>
--- a/Project Schedle.xlsx
+++ b/Project Schedle.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Welldy\private\PROJECT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Welldy\private\PROJECT\airlangga-admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15510" windowHeight="3340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15510" windowHeight="3340" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Schedule" sheetId="1" r:id="rId1"/>
+    <sheet name="31-05" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>JUNI</t>
   </si>
@@ -84,6 +85,48 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>Facility Bugs Insert Data</t>
+  </si>
+  <si>
+    <t>Hanya Item Ke 2 saya yang masuk Note Fasilitasnya</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Root Cause/Analisa Sementara</t>
+  </si>
+  <si>
+    <t>INSERT NEW PACKAGE TOUR</t>
+  </si>
+  <si>
+    <t>Binding Image Caption</t>
+  </si>
+  <si>
+    <t>Add Time Travel</t>
+  </si>
+  <si>
+    <t>tambah waktu acara</t>
+  </si>
+  <si>
+    <t>dynamic datepicker</t>
+  </si>
+  <si>
+    <t>binding note image input ke image view</t>
+  </si>
+  <si>
+    <t>Set Default Video</t>
+  </si>
+  <si>
+    <t>setting default video ketika kosong</t>
   </si>
 </sst>
 </file>
@@ -166,20 +209,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,7 +508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C8:BB27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
@@ -476,70 +522,70 @@
   </cols>
   <sheetData>
     <row r="8" spans="3:54" x14ac:dyDescent="0.35">
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-      <c r="AA8" s="2"/>
-      <c r="AB8" s="2"/>
-      <c r="AC8" s="2"/>
-      <c r="AD8" s="2"/>
-      <c r="AE8" s="2"/>
-      <c r="AF8" s="2"/>
-      <c r="AG8" s="2"/>
-      <c r="AH8" s="2"/>
-      <c r="AI8" s="2" t="s">
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="4"/>
+      <c r="AB8" s="4"/>
+      <c r="AC8" s="4"/>
+      <c r="AD8" s="4"/>
+      <c r="AE8" s="4"/>
+      <c r="AF8" s="4"/>
+      <c r="AG8" s="4"/>
+      <c r="AH8" s="4"/>
+      <c r="AI8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AJ8" s="2"/>
-      <c r="AK8" s="2"/>
-      <c r="AL8" s="2"/>
-      <c r="AM8" s="2"/>
-      <c r="AN8" s="2"/>
-      <c r="AO8" s="2"/>
-      <c r="AP8" s="2"/>
-      <c r="AQ8" s="2"/>
-      <c r="AR8" s="2"/>
-      <c r="AS8" s="2"/>
-      <c r="AT8" s="2"/>
-      <c r="AU8" s="2"/>
-      <c r="AV8" s="2"/>
-      <c r="AW8" s="2"/>
-      <c r="AX8" s="2"/>
-      <c r="AY8" s="2"/>
-      <c r="AZ8" s="2"/>
-      <c r="BA8" s="2"/>
-      <c r="BB8" s="2"/>
+      <c r="AJ8" s="4"/>
+      <c r="AK8" s="4"/>
+      <c r="AL8" s="4"/>
+      <c r="AM8" s="4"/>
+      <c r="AN8" s="4"/>
+      <c r="AO8" s="4"/>
+      <c r="AP8" s="4"/>
+      <c r="AQ8" s="4"/>
+      <c r="AR8" s="4"/>
+      <c r="AS8" s="4"/>
+      <c r="AT8" s="4"/>
+      <c r="AU8" s="4"/>
+      <c r="AV8" s="4"/>
+      <c r="AW8" s="4"/>
+      <c r="AX8" s="4"/>
+      <c r="AY8" s="4"/>
+      <c r="AZ8" s="4"/>
+      <c r="BA8" s="4"/>
+      <c r="BB8" s="4"/>
     </row>
     <row r="9" spans="3:54" x14ac:dyDescent="0.35">
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="1">
         <v>1</v>
       </c>
@@ -692,34 +738,34 @@
       </c>
     </row>
     <row r="10" spans="3:54" x14ac:dyDescent="0.35">
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="6"/>
-      <c r="AB10" s="6"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
       <c r="AE10" s="1"/>
@@ -754,8 +800,8 @@
       <c r="D11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -814,7 +860,7 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="6"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -873,9 +919,9 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -934,9 +980,9 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -995,9 +1041,9 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
@@ -1056,9 +1102,9 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
@@ -1117,7 +1163,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
-      <c r="T17" s="6"/>
+      <c r="T17" s="3"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
@@ -1176,8 +1222,8 @@
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
-      <c r="U18" s="6"/>
-      <c r="V18" s="6"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
@@ -1236,9 +1282,9 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
-      <c r="W19" s="6"/>
-      <c r="X19" s="6"/>
-      <c r="Y19" s="6"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
@@ -1294,10 +1340,10 @@
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-      <c r="Z20" s="6"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="3"/>
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
@@ -1352,11 +1398,11 @@
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
       <c r="Z21" s="1"/>
-      <c r="AA21" s="6"/>
+      <c r="AA21" s="3"/>
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
@@ -1386,10 +1432,10 @@
       <c r="BB21" s="1"/>
     </row>
     <row r="22" spans="3:54" x14ac:dyDescent="0.35">
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="4"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1413,17 +1459,17 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
-      <c r="AB22" s="6"/>
-      <c r="AC22" s="6"/>
-      <c r="AD22" s="6"/>
-      <c r="AE22" s="6"/>
-      <c r="AF22" s="6"/>
-      <c r="AG22" s="6"/>
-      <c r="AH22" s="6"/>
-      <c r="AI22" s="6"/>
-      <c r="AJ22" s="6"/>
-      <c r="AK22" s="6"/>
-      <c r="AL22" s="6"/>
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="3"/>
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="3"/>
+      <c r="AG22" s="3"/>
+      <c r="AH22" s="3"/>
+      <c r="AI22" s="3"/>
+      <c r="AJ22" s="3"/>
+      <c r="AK22" s="3"/>
+      <c r="AL22" s="3"/>
       <c r="AM22" s="1"/>
       <c r="AN22" s="1"/>
       <c r="AO22" s="1"/>
@@ -1471,8 +1517,8 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
-      <c r="AB23" s="6"/>
-      <c r="AC23" s="6"/>
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="3"/>
       <c r="AD23" s="1"/>
       <c r="AE23" s="1"/>
       <c r="AF23" s="1"/>
@@ -1531,8 +1577,8 @@
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
-      <c r="AD24" s="6"/>
-      <c r="AE24" s="6"/>
+      <c r="AD24" s="3"/>
+      <c r="AE24" s="3"/>
       <c r="AF24" s="1"/>
       <c r="AG24" s="1"/>
       <c r="AH24" s="1"/>
@@ -1591,7 +1637,7 @@
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
       <c r="AE25" s="1"/>
-      <c r="AF25" s="6"/>
+      <c r="AF25" s="3"/>
       <c r="AG25" s="1"/>
       <c r="AH25" s="1"/>
       <c r="AI25" s="1"/>
@@ -1650,9 +1696,9 @@
       <c r="AD26" s="1"/>
       <c r="AE26" s="1"/>
       <c r="AF26" s="1"/>
-      <c r="AG26" s="6"/>
-      <c r="AH26" s="6"/>
-      <c r="AI26" s="6"/>
+      <c r="AG26" s="3"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="3"/>
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
       <c r="AL26" s="1"/>
@@ -1711,9 +1757,9 @@
       <c r="AG27" s="1"/>
       <c r="AH27" s="1"/>
       <c r="AI27" s="1"/>
-      <c r="AJ27" s="6"/>
-      <c r="AK27" s="6"/>
-      <c r="AL27" s="6"/>
+      <c r="AJ27" s="3"/>
+      <c r="AK27" s="3"/>
+      <c r="AL27" s="3"/>
       <c r="AM27" s="1"/>
       <c r="AN27" s="1"/>
       <c r="AO27" s="1"/>
@@ -1742,4 +1788,137 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="3.90625" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="D4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D4:G4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
LOAD IMAGE FROM STORAGE
</commit_message>
<xml_diff>
--- a/Project Schedle.xlsx
+++ b/Project Schedle.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Welldy\private\PROJECT\airlangga-admin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT\AIRLANGGA\airlangga-admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E0B9F9-B391-417D-BCBE-3DD39514C14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15510" windowHeight="3340" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>JUNI</t>
   </si>
@@ -127,12 +128,33 @@
   </si>
   <si>
     <t>setting default video ketika kosong</t>
+  </si>
+  <si>
+    <t>filter redudance array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remove duplidate date </t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>cheking file type</t>
+  </si>
+  <si>
+    <t>file type must be jpg/png</t>
+  </si>
+  <si>
+    <t>Note Loop Image</t>
+  </si>
+  <si>
+    <t>UPDATE PACKAGE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -142,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +174,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -209,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -226,6 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,23 +534,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C8:BB27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="5.08984375" customWidth="1"/>
-    <col min="4" max="4" width="21.54296875" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
     <col min="5" max="33" width="4" customWidth="1"/>
-    <col min="34" max="40" width="4.08984375" customWidth="1"/>
-    <col min="41" max="54" width="4.36328125" customWidth="1"/>
+    <col min="34" max="40" width="4.140625" customWidth="1"/>
+    <col min="41" max="54" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
@@ -583,7 +612,7 @@
       <c r="BA8" s="4"/>
       <c r="BB8" s="4"/>
     </row>
-    <row r="9" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="1">
@@ -737,7 +766,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
         <v>1</v>
       </c>
@@ -793,7 +822,7 @@
       <c r="BA10" s="1"/>
       <c r="BB10" s="1"/>
     </row>
-    <row r="11" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
         <v>1</v>
       </c>
@@ -851,7 +880,7 @@
       <c r="BA11" s="1"/>
       <c r="BB11" s="1"/>
     </row>
-    <row r="12" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C12" s="1">
         <v>2</v>
       </c>
@@ -909,7 +938,7 @@
       <c r="BA12" s="1"/>
       <c r="BB12" s="1"/>
     </row>
-    <row r="13" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C13" s="1">
         <v>3</v>
       </c>
@@ -967,7 +996,7 @@
       <c r="BA13" s="1"/>
       <c r="BB13" s="1"/>
     </row>
-    <row r="14" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C14" s="1">
         <v>4</v>
       </c>
@@ -1025,7 +1054,7 @@
       <c r="BA14" s="1"/>
       <c r="BB14" s="1"/>
     </row>
-    <row r="15" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C15" s="1">
         <v>5</v>
       </c>
@@ -1083,7 +1112,7 @@
       <c r="BA15" s="1"/>
       <c r="BB15" s="1"/>
     </row>
-    <row r="16" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C16" s="1">
         <v>6</v>
       </c>
@@ -1141,7 +1170,7 @@
       <c r="BA16" s="1"/>
       <c r="BB16" s="1"/>
     </row>
-    <row r="17" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
         <v>7</v>
       </c>
@@ -1199,7 +1228,7 @@
       <c r="BA17" s="1"/>
       <c r="BB17" s="1"/>
     </row>
-    <row r="18" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
         <v>8</v>
       </c>
@@ -1257,7 +1286,7 @@
       <c r="BA18" s="1"/>
       <c r="BB18" s="1"/>
     </row>
-    <row r="19" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
         <v>9</v>
       </c>
@@ -1315,7 +1344,7 @@
       <c r="BA19" s="1"/>
       <c r="BB19" s="1"/>
     </row>
-    <row r="20" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <v>10</v>
       </c>
@@ -1373,7 +1402,7 @@
       <c r="BA20" s="1"/>
       <c r="BB20" s="1"/>
     </row>
-    <row r="21" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <v>12</v>
       </c>
@@ -1431,7 +1460,7 @@
       <c r="BA21" s="1"/>
       <c r="BB21" s="1"/>
     </row>
-    <row r="22" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
@@ -1487,7 +1516,7 @@
       <c r="BA22" s="1"/>
       <c r="BB22" s="1"/>
     </row>
-    <row r="23" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <v>11</v>
       </c>
@@ -1545,7 +1574,7 @@
       <c r="BA23" s="1"/>
       <c r="BB23" s="1"/>
     </row>
-    <row r="24" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <v>12</v>
       </c>
@@ -1603,7 +1632,7 @@
       <c r="BA24" s="1"/>
       <c r="BB24" s="1"/>
     </row>
-    <row r="25" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <v>13</v>
       </c>
@@ -1661,7 +1690,7 @@
       <c r="BA25" s="1"/>
       <c r="BB25" s="1"/>
     </row>
-    <row r="26" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
         <v>14</v>
       </c>
@@ -1719,7 +1748,7 @@
       <c r="BA26" s="1"/>
       <c r="BB26" s="1"/>
     </row>
-    <row r="27" spans="3:54" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
         <v>15</v>
       </c>
@@ -1791,22 +1820,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:G17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="C4:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="3.90625" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.90625" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D4" s="7" t="s">
         <v>26</v>
       </c>
@@ -1814,7 +1843,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>22</v>
       </c>
@@ -1828,7 +1857,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>1</v>
       </c>
@@ -1839,7 +1868,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>2</v>
       </c>
@@ -1850,7 +1879,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>3</v>
       </c>
@@ -1863,8 +1892,11 @@
       <c r="F8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="G8" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>4</v>
       </c>
@@ -1875,49 +1907,78 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>12</v>
       </c>
     </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D19:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>